<commit_message>
Fix bridge rectifier link in BOM
</commit_message>
<xml_diff>
--- a/Bill Of Material.xlsx
+++ b/Bill Of Material.xlsx
@@ -178,7 +178,7 @@
     <t xml:space="preserve">Diyot Köprü, 25A 600V (min)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.robotistan.com/gbj2510-25-a-1000-v-kopru-diyot</t>
+    <t xml:space="preserve">https://www.direnc.net/35a-1000v-kopru-diyot-lehimlemeye-uygun</t>
   </si>
   <si>
     <t xml:space="preserve">Heat sink (diode bridge)</t>
@@ -278,6 +278,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -299,6 +300,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -464,10 +466,10 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="37.63"/>
@@ -1081,7 +1083,7 @@
     <hyperlink ref="F14" r:id="rId12" display="https://www.direnc.net/33-ohm-25w-aluminyum-direnc"/>
     <hyperlink ref="F15" r:id="rId13" display="https://www.direnc.net/220k-potans"/>
     <hyperlink ref="F16" r:id="rId14" display="https://www.direnc.net/drn-302-beyaz-pot-basligi"/>
-    <hyperlink ref="F19" r:id="rId15" display="https://www.robotistan.com/gbj2510-25-a-1000-v-kopru-diyot"/>
+    <hyperlink ref="F19" r:id="rId15" display="https://www.direnc.net/35a-1000v-kopru-diyot-lehimlemeye-uygun"/>
     <hyperlink ref="F24" r:id="rId16" display="https://www.direnc.net/bta26-600--600v-25a-4-quadrant-logic-level-triac"/>
     <hyperlink ref="F29" r:id="rId17" display="https://www.direnc.net/db3-diac-36v-do-35"/>
     <hyperlink ref="F31" r:id="rId18" display="https://www.direnc.net/kts102-on-off-3-ayak-toggle"/>

</xml_diff>